<commit_message>
Queue Report sequence added. One Drive folder is now dynamic. Adds Queue Report and Faulty Bills automatically to PC's One Drive folder. Some excel actions added.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OguzhanTasgin\Documents\UiPath\Bill Of Lading Processing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752AF950-32FF-4850-9AFA-4CF0E6F4CEEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7319295-0D2E-4EE6-A716-2F8BB0FB9814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="3960" windowWidth="21285" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -129,13 +129,22 @@
     <t>Bills Folder</t>
   </si>
   <si>
-    <t>OneDriveLocation</t>
-  </si>
-  <si>
     <t xml:space="preserve">OneDrive folder location where Faulty Bills will be saved. </t>
   </si>
   <si>
-    <t>C:\Users\OguzhanTasgin\OneDrive - PRP Business Solutions\FaultyBills\</t>
+    <t>OrchestratorCredential</t>
+  </si>
+  <si>
+    <t>Orchestrator Credential</t>
+  </si>
+  <si>
+    <t>Orchestrator platform username and password.</t>
+  </si>
+  <si>
+    <t>One Drive Folder Name</t>
+  </si>
+  <si>
+    <t>OneDrive - PRP Business Solutions</t>
   </si>
 </sst>
 </file>
@@ -525,7 +534,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -583,13 +592,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
@@ -614,7 +623,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>